<commit_message>
add displayDate to excel templates
</commit_message>
<xml_diff>
--- a/ExceltoMODSWF/archival-mods-template-enhanced.xlsx
+++ b/ExceltoMODSWF/archival-mods-template-enhanced.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goslen\Git\Metadata-Miscellany\DCR_MODS_templates\ExceltoMODSWF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goslen\git_repos\box-c-mods-templates\ExceltoMODSWF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5776E90D-089C-4ECC-B6D8-489FE96876EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22178C2C-A6F1-4EB1-9E75-C76867C2ABAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="1425" windowWidth="25980" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2130" yWindow="1575" windowWidth="25575" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Template" sheetId="1" r:id="rId1"/>
+    <sheet name="Guide" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;&lt;bulkMetadata&gt;</t>
   </si>
@@ -66,15 +67,6 @@
     <t>Accession Number</t>
   </si>
   <si>
-    <t>&lt;mods:originInfo&gt;&lt;mods:dateCreated encoding="edtf"&gt;</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>&lt;/mods:dateCreated&gt;&lt;/mods:originInfo&gt;</t>
-  </si>
-  <si>
     <t>&lt;mods:relatedItem type="original"&gt;&lt;mods:identifier displayLabel="Source Media Identifier"&gt;</t>
   </si>
   <si>
@@ -103,6 +95,51 @@
   </si>
   <si>
     <t>&lt;mods:note displayLabel="Description"&gt;</t>
+  </si>
+  <si>
+    <t>Date Created</t>
+  </si>
+  <si>
+    <t>&lt;mods:dateCreated encoding="edtf"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mods:originInfo&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/mods:originInfo&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/mods:dateCreated&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mods:displayDate&gt;</t>
+  </si>
+  <si>
+    <t>Display Date</t>
+  </si>
+  <si>
+    <t>&lt;/mods:displayDate&gt;</t>
+  </si>
+  <si>
+    <t>Field Label</t>
+  </si>
+  <si>
+    <t>Notes and Best Practices</t>
+  </si>
+  <si>
+    <t>Date of creation of the resource, encoded according to EDTF. See https://adminliveunc.sharepoint.com/sites/DigitalCollectionsDocumentation/SitePages/Date-metadata-in-DCR.aspx for help and additional resources</t>
+  </si>
+  <si>
+    <t>Optional free text date field that allows a date to be represented in human-readable form. It is recommended that mods:displayDate be entered to complement mods:dateCreated in order to provide a human-readable equivalent to the EDTF date. If you are unable to provide an EDTF date, providing only a mods:displayDate is preferable to no date.</t>
+  </si>
+  <si>
+    <t>DCR Object ID</t>
+  </si>
+  <si>
+    <t>Accession number</t>
+  </si>
+  <si>
+    <t>5-digit archival collection number. "70096"</t>
   </si>
 </sst>
 </file>
@@ -169,15 +206,15 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,116 +529,242 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" customWidth="1"/>
-    <col min="17" max="17" width="22.28515625" customWidth="1"/>
-    <col min="20" max="20" width="22.28515625" customWidth="1"/>
-    <col min="23" max="23" width="31" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="22.28515625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="2"/>
+    <col min="8" max="8" width="20.85546875" style="2" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="2"/>
+    <col min="11" max="11" width="22.28515625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="2"/>
+    <col min="13" max="14" width="9.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" style="2" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="22.28515625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="2" customWidth="1"/>
+    <col min="20" max="21" width="9.140625" style="2"/>
+    <col min="22" max="22" width="22.28515625" style="2" customWidth="1"/>
+    <col min="23" max="24" width="9.140625" style="2"/>
+    <col min="25" max="25" width="22.28515625" style="2" customWidth="1"/>
+    <col min="26" max="27" width="9.140625" style="2"/>
+    <col min="28" max="28" width="31" style="2" customWidth="1"/>
+    <col min="29" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="P2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="AA2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="S2" t="s">
+      <c r="AC2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U2" t="s">
-        <v>8</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="W2" s="7" t="s">
+      <c r="AD2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="X2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="Q3" s="5"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="V3" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8150A89C-496C-486D-B112-981F8479AA17}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="58.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100060CAEA771823F4F9BA21EE45585473F" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c823f7b768b656f654f262873a6854f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81007de4-ee29-48be-8634-4fbb6dd6f763" xmlns:ns3="fdb5634d-e10a-4de6-afed-2492c365d474" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fd052af535147c2bf9c2ace5143a7237" ns2:_="" ns3:_="">
     <xsd:import namespace="81007de4-ee29-48be-8634-4fbb6dd6f763"/>
@@ -818,22 +981,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2218DF2E-8B03-41C5-82BD-4E07ED3AC316}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48E12C0E-954A-4EBF-8B0C-CA38C7369109}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C1DB513-A53A-428B-AA1B-CA693350680F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -850,21 +1015,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48E12C0E-954A-4EBF-8B0C-CA38C7369109}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2218DF2E-8B03-41C5-82BD-4E07ED3AC316}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>